<commit_message>
Surgical indication stuff done differently. Not many cases!
</commit_message>
<xml_diff>
--- a/tables_3_18_24.xlsx
+++ b/tables_3_18_24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpishar\Desktop\eoa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F698639C-5851-45E0-B2EB-111F10000278}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ACE3EB-1BF9-439C-98A4-2387293BA181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="5" xr2:uid="{B3DBD4D2-3816-4F19-905B-1249A3A8CC5C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="6" xr2:uid="{B3DBD4D2-3816-4F19-905B-1249A3A8CC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Elix" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="159">
   <si>
     <t>Table: Descriptive statistics</t>
   </si>
@@ -504,13 +505,31 @@
   <si>
     <t>51 (0.4%)</t>
   </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Post-traumatic</t>
+  </si>
+  <si>
+    <t>Inflammatory</t>
+  </si>
+  <si>
+    <t>Arthritis, type unspecified</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -693,13 +712,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -708,9 +723,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -743,33 +755,69 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -777,44 +825,21 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,135 +1168,135 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="5" spans="3:7" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="10"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="3:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1303,363 +1328,363 @@
   <sheetData>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:9" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="39"/>
+      <c r="E6" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="40"/>
+      <c r="G6" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="2:9" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B8" s="18">
+      <c r="B8" s="15">
         <v>2009</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="15">
         <v>39820</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="15">
         <v>0.84</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="15">
         <v>28296</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="15">
         <v>1.01</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="15">
         <v>68116</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="15">
         <v>0.91</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
+      <c r="B9" s="15">
         <v>2010</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="15">
         <v>38271</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="15">
         <v>0.99</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="15">
         <v>31947</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="15">
         <v>1.05</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="15">
         <v>70218</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
         <v>1.02</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
+      <c r="B10" s="15">
         <v>2011</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="15">
         <v>40555</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="15">
         <v>0.86</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="15">
         <v>35917</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="15">
         <v>0.98</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="15">
         <v>76472</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="15">
         <v>0.92</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
+      <c r="B11" s="15">
         <v>2012</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="15">
         <v>39097</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="15">
         <v>0.98</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="15">
         <v>36171</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="15">
         <v>0.97</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="15">
         <v>75268</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="15">
         <v>0.98</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B12" s="18">
+      <c r="B12" s="15">
         <v>2013</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="15">
         <v>32369</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="15">
         <v>0.93</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="15">
         <v>31559</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="15">
         <v>1.03</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="15">
         <v>63928</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="15">
         <v>0.98</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B13" s="18">
+      <c r="B13" s="15">
         <v>2014</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="15">
         <v>31859</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="15">
         <v>0.91</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="15">
         <v>33497</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="15">
         <v>1.04</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="15">
         <v>65356</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="15">
         <v>0.98</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B14" s="18">
+      <c r="B14" s="15">
         <v>2015</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="15">
         <v>19825</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="15">
         <v>23102</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="15">
         <v>1.22</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="15">
         <v>42927</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="15">
         <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B15" s="18">
+      <c r="B15" s="15">
         <v>2016</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="15">
         <v>22723</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="15">
         <v>1.17</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="15">
         <v>28288</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="15">
         <v>1.5</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="15">
         <v>51011</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="15">
         <v>1.35</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B16" s="18">
+      <c r="B16" s="15">
         <v>2017</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="15">
         <v>18837</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="15">
         <v>1.39</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="15">
         <v>24870</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="15">
         <v>1.86</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="15">
         <v>43707</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="15">
         <v>1.66</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B17" s="18">
+      <c r="B17" s="15">
         <v>2018</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="15">
         <v>18013</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>2.02</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="15">
         <v>23805</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="15">
         <v>2.66</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="15">
         <v>41818</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="15">
         <v>2.38</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="18">
+      <c r="B18" s="15">
         <v>2019</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="15">
         <v>13447</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="15">
         <v>2.75</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="15">
         <v>18780</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="15">
         <v>3.78</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="15">
         <v>32227</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="15">
         <v>3.35</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="18">
+      <c r="B19" s="15">
         <v>2020</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="15">
         <v>13184</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="15">
         <v>3.66</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="15">
         <v>17182</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="15">
         <v>5.28</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="15">
         <v>30366</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="15">
         <v>4.58</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B20" s="18">
+      <c r="B20" s="15">
         <v>2021</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="15">
         <v>14786</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="15">
         <v>5.31</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="15">
         <v>19878</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="15">
         <v>7.67</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="15">
         <v>34664</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="15">
         <v>6.66</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="18">
+      <c r="B21" s="15">
         <v>2022</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="15">
         <v>6838</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="15">
         <v>6.6</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="15">
         <v>9296</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="15">
         <v>8.9499999999999993</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="15">
         <v>16134</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="15">
         <v>7.95</v>
       </c>
     </row>
@@ -1684,265 +1709,265 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="8" spans="3:10" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="18">
+      <c r="C9" s="15">
         <v>2009</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="15">
         <v>0.91</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="18">
+      <c r="C10" s="15">
         <v>2010</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="15">
         <v>1.02</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="11"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="3:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="C11" s="18">
+      <c r="C11" s="15">
         <v>2011</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="15">
         <v>0.92</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="18">
+      <c r="C12" s="15">
         <v>2012</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="15">
         <v>0.98</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+      <c r="C13" s="15">
         <v>2013</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="15">
         <v>0.98</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="18">
+      <c r="C14" s="15">
         <v>2014</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="15">
         <v>0.98</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="18">
+      <c r="C15" s="15">
         <v>2015</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="15">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="18">
+      <c r="C16" s="15">
         <v>2016</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="15">
         <v>1.35</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="18">
+      <c r="C17" s="15">
         <v>2017</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>1.66</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="18">
+      <c r="C18" s="15">
         <v>2018</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="15">
         <v>2.38</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="18">
+      <c r="C19" s="15">
         <v>2019</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="15">
         <v>3.35</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="18">
+      <c r="C20" s="15">
         <v>2020</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="15">
         <v>4.58</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="10">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="18">
+      <c r="C21" s="15">
         <v>2021</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="15">
         <v>6.66</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="3:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="18">
+      <c r="C22" s="15">
         <v>2022</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="15">
         <v>7.95</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G23" s="13">
+      <c r="G23" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G24" s="13">
+      <c r="G24" s="10">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G25" s="13">
+      <c r="G25" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="13">
+      <c r="G26" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="13">
+      <c r="G27" s="10">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="13">
+      <c r="G28" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G29" s="13">
+      <c r="G29" s="10">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="13">
+      <c r="G30" s="10">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G31" s="13">
+      <c r="G31" s="10">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="13">
+      <c r="G32" s="10">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G33" s="13">
+      <c r="G33" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="13">
+      <c r="G34" s="10">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G35" s="13">
+      <c r="G35" s="10">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="13">
+      <c r="G36" s="10">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="13">
+      <c r="G37" s="10">
         <v>26</v>
       </c>
     </row>
     <row r="38" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="13">
+      <c r="G38" s="10">
         <v>27</v>
       </c>
     </row>
     <row r="39" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G39" s="13">
+      <c r="G39" s="10">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G40" s="13">
+      <c r="G40" s="10">
         <v>29</v>
       </c>
     </row>
     <row r="41" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G41" s="13">
+      <c r="G41" s="10">
         <v>30</v>
       </c>
     </row>
     <row r="42" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G42" s="13">
+      <c r="G42" s="10">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G43" s="13">
+      <c r="G43" s="10">
         <v>32</v>
       </c>
     </row>
@@ -1967,38 +1992,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="26">
+      <c r="B1" s="21">
         <v>503373</v>
       </c>
-      <c r="C1" s="27">
-        <f>B1/712212</f>
+      <c r="C1" s="22">
+        <f t="shared" ref="C1:C32" si="0">B1/712212</f>
         <v>0.70677410658624118</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="11">
         <v>235506</v>
       </c>
-      <c r="C2" s="24">
-        <f>B2/712212</f>
+      <c r="C2" s="19">
+        <f t="shared" si="0"/>
         <v>0.33066839648868596</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="11">
         <v>212312</v>
       </c>
-      <c r="C3" s="24">
-        <f>B3/712212</f>
+      <c r="C3" s="19">
+        <f t="shared" si="0"/>
         <v>0.29810225045351663</v>
       </c>
       <c r="E3" t="s">
@@ -2006,357 +2031,357 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>171198</v>
       </c>
-      <c r="C4" s="24">
-        <f>B4/712212</f>
+      <c r="C4" s="19">
+        <f t="shared" si="0"/>
         <v>0.24037505686509072</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>140356</v>
       </c>
-      <c r="C5" s="24">
-        <f>B5/712212</f>
+      <c r="C5" s="19">
+        <f t="shared" si="0"/>
         <v>0.19707053517772799</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>129838</v>
       </c>
-      <c r="C6" s="24">
-        <f>B6/712212</f>
+      <c r="C6" s="19">
+        <f t="shared" si="0"/>
         <v>0.18230246050333326</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>128816</v>
       </c>
-      <c r="C7" s="24">
-        <f>B7/712212</f>
+      <c r="C7" s="19">
+        <f t="shared" si="0"/>
         <v>0.18086749451006162</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>124279</v>
       </c>
-      <c r="C8" s="24">
-        <f>B8/712212</f>
+      <c r="C8" s="19">
+        <f t="shared" si="0"/>
         <v>0.17449720027182916</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>76171</v>
       </c>
-      <c r="C9" s="24">
-        <f>B9/712212</f>
+      <c r="C9" s="19">
+        <f t="shared" si="0"/>
         <v>0.10694989694079853</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>65571</v>
       </c>
-      <c r="C10" s="24">
-        <f>B10/712212</f>
+      <c r="C10" s="19">
+        <f t="shared" si="0"/>
         <v>9.2066688008626649E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>62057</v>
       </c>
-      <c r="C11" s="24">
-        <f>B11/712212</f>
+      <c r="C11" s="19">
+        <f t="shared" si="0"/>
         <v>8.7132763839980226E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>57464</v>
       </c>
-      <c r="C12" s="24">
-        <f>B12/712212</f>
+      <c r="C12" s="19">
+        <f t="shared" si="0"/>
         <v>8.0683841328143865E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>55019</v>
       </c>
-      <c r="C13" s="24">
-        <f>B13/712212</f>
+      <c r="C13" s="19">
+        <f t="shared" si="0"/>
         <v>7.725087473954384E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>52241</v>
       </c>
-      <c r="C14" s="24">
-        <f>B14/712212</f>
+      <c r="C14" s="19">
+        <f t="shared" si="0"/>
         <v>7.335035073826332E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="11">
         <v>50214</v>
       </c>
-      <c r="C15" s="24">
-        <f>B15/712212</f>
+      <c r="C15" s="19">
+        <f t="shared" si="0"/>
         <v>7.0504288049064043E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="11">
         <v>41415</v>
       </c>
-      <c r="C16" s="24">
-        <f>B16/712212</f>
+      <c r="C16" s="19">
+        <f t="shared" si="0"/>
         <v>5.8149820559047029E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="11">
         <v>36763</v>
       </c>
-      <c r="C17" s="24">
-        <f>B17/712212</f>
+      <c r="C17" s="19">
+        <f t="shared" si="0"/>
         <v>5.161805754466367E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="11">
         <v>35186</v>
       </c>
-      <c r="C18" s="24">
-        <f>B18/712212</f>
+      <c r="C18" s="19">
+        <f t="shared" si="0"/>
         <v>4.9403829196924515E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="11">
         <v>28682</v>
       </c>
-      <c r="C19" s="24">
-        <f>B19/712212</f>
+      <c r="C19" s="19">
+        <f t="shared" si="0"/>
         <v>4.0271716848354143E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="11">
         <v>27578</v>
       </c>
-      <c r="C20" s="24">
-        <f>B20/712212</f>
+      <c r="C20" s="19">
+        <f t="shared" si="0"/>
         <v>3.8721616597305296E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="11">
         <v>20537</v>
       </c>
-      <c r="C21" s="24">
-        <f>B21/712212</f>
+      <c r="C21" s="19">
+        <f t="shared" si="0"/>
         <v>2.8835515267925844E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="11">
         <v>15890</v>
       </c>
-      <c r="C22" s="24">
-        <f>B22/712212</f>
+      <c r="C22" s="19">
+        <f t="shared" si="0"/>
         <v>2.2310772635114263E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="11">
         <v>12653</v>
       </c>
-      <c r="C23" s="24">
-        <f>B23/712212</f>
+      <c r="C23" s="19">
+        <f t="shared" si="0"/>
         <v>1.7765777605544417E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="11">
         <v>10873</v>
       </c>
-      <c r="C24" s="24">
-        <f>B24/712212</f>
+      <c r="C24" s="19">
+        <f t="shared" si="0"/>
         <v>1.5266521765991026E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="11">
         <v>9971</v>
       </c>
-      <c r="C25" s="24">
-        <f>B25/712212</f>
+      <c r="C25" s="19">
+        <f t="shared" si="0"/>
         <v>1.400004493044206E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="11">
         <v>9550</v>
       </c>
-      <c r="C26" s="24">
-        <f>B26/712212</f>
+      <c r="C26" s="19">
+        <f t="shared" si="0"/>
         <v>1.3408928802098251E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="11">
         <v>7153</v>
       </c>
-      <c r="C27" s="24">
-        <f>B27/712212</f>
+      <c r="C27" s="19">
+        <f t="shared" si="0"/>
         <v>1.0043357876587309E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="11">
         <v>4550</v>
       </c>
-      <c r="C28" s="24">
-        <f>B28/712212</f>
+      <c r="C28" s="19">
+        <f t="shared" si="0"/>
         <v>6.3885472303190621E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="11">
         <v>4115</v>
       </c>
-      <c r="C29" s="24">
-        <f>B29/712212</f>
+      <c r="C29" s="19">
+        <f t="shared" si="0"/>
         <v>5.777774033574273E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="11">
         <v>3499</v>
       </c>
-      <c r="C30" s="24">
-        <f>B30/712212</f>
+      <c r="C30" s="19">
+        <f t="shared" si="0"/>
         <v>4.9128630239310767E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="11">
         <v>2061</v>
       </c>
-      <c r="C31" s="24">
-        <f>B31/712212</f>
+      <c r="C31" s="19">
+        <f t="shared" si="0"/>
         <v>2.893801283887382E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="11">
         <v>549</v>
       </c>
-      <c r="C32" s="24">
-        <f>B32/712212</f>
+      <c r="C32" s="19">
+        <f t="shared" si="0"/>
         <v>7.7083789658135497E-4</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A1:C33">
@@ -2384,231 +2409,231 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="2:6" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="32"/>
-      <c r="C7" s="33" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="45" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="35"/>
-      <c r="C8" s="36" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="31">
         <v>0.53500000000000003</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="31">
         <v>0.19</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="31">
         <v>0.54400000000000004</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="31">
         <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="42">
+      <c r="F14" s="31">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="42">
+      <c r="F19" s="31">
         <v>0.92100000000000004</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="29"/>
+      <c r="F20" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2624,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4966FD-1D6D-4A84-812B-352D48CD3902}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,312 +2663,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="41.25" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="33" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="15"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="45"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="15"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="28">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="28">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="28">
         <v>0.01</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="39">
+      <c r="E15" s="28">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="39">
+      <c r="E16" s="28">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="39">
+      <c r="E17" s="28">
         <v>1.4500000000000001E-2</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="46"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2952,4 +2977,484 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4464D4A-37E4-4425-8740-6C871D1B96A5}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="48"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2009</v>
+      </c>
+      <c r="B3">
+        <v>46619</v>
+      </c>
+      <c r="C3" s="19">
+        <v>9.9699999999999997E-3</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3" s="19">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>88</v>
+      </c>
+      <c r="G3" s="19">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>21459</v>
+      </c>
+      <c r="I3" s="19">
+        <v>7.3600000000000002E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4">
+        <v>48667</v>
+      </c>
+      <c r="C4" s="19">
+        <v>1.03E-2</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>73</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>21527</v>
+      </c>
+      <c r="I4" s="19">
+        <v>9.8899999999999995E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2011</v>
+      </c>
+      <c r="B5">
+        <v>52850</v>
+      </c>
+      <c r="C5" s="19">
+        <v>8.8199999999999997E-3</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="E5" s="19">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="F5">
+        <v>99</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>23583</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2012</v>
+      </c>
+      <c r="B6">
+        <v>51589</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="19">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>83</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H6">
+        <v>23657</v>
+      </c>
+      <c r="I6" s="19">
+        <v>9.1699999999999993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2013</v>
+      </c>
+      <c r="B7">
+        <v>43253</v>
+      </c>
+      <c r="C7" s="19">
+        <v>9.7099999999999999E-3</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7" s="19">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>93</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>20639</v>
+      </c>
+      <c r="I7" s="19">
+        <v>9.9799999999999993E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2014</v>
+      </c>
+      <c r="B8">
+        <v>44255</v>
+      </c>
+      <c r="C8" s="19">
+        <v>9.4500000000000001E-3</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>127</v>
+      </c>
+      <c r="G8" s="19">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>21050</v>
+      </c>
+      <c r="I8" s="19">
+        <v>1.04E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2015</v>
+      </c>
+      <c r="B9">
+        <v>33526</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" s="19">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>56</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="H9">
+        <v>9379</v>
+      </c>
+      <c r="I9" s="19">
+        <v>1.18E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2016</v>
+      </c>
+      <c r="B10">
+        <v>50992</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1.35E-2</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2017</v>
+      </c>
+      <c r="B11">
+        <v>43686</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>30</v>
+      </c>
+      <c r="G11" s="19">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2018</v>
+      </c>
+      <c r="B12">
+        <v>41792</v>
+      </c>
+      <c r="C12" s="19">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="F12">
+        <v>42</v>
+      </c>
+      <c r="G12" s="19">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2019</v>
+      </c>
+      <c r="B13">
+        <v>32214</v>
+      </c>
+      <c r="C13" s="19">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0.08</v>
+      </c>
+      <c r="F13">
+        <v>17</v>
+      </c>
+      <c r="G13" s="19">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2020</v>
+      </c>
+      <c r="B14">
+        <v>30357</v>
+      </c>
+      <c r="C14" s="19">
+        <v>4.58E-2</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14" s="19">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2021</v>
+      </c>
+      <c r="B15">
+        <v>34654</v>
+      </c>
+      <c r="C15" s="19">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+      <c r="E15" s="19">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>21</v>
+      </c>
+      <c r="G15" s="19">
+        <v>0.19</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2022</v>
+      </c>
+      <c r="B16">
+        <v>16130</v>
+      </c>
+      <c r="C16" s="19">
+        <v>7.9500000000000001E-2</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0.182</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0.125</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated some checks -- minor.
</commit_message>
<xml_diff>
--- a/tables_3_18_24.xlsx
+++ b/tables_3_18_24.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpishar\Desktop\eoa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ACE3EB-1BF9-439C-98A4-2387293BA181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDB55B7-FF03-426B-BFDE-C5332ED0A3DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="6" xr2:uid="{B3DBD4D2-3816-4F19-905B-1249A3A8CC5C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="4" activeTab="7" xr2:uid="{B3DBD4D2-3816-4F19-905B-1249A3A8CC5C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Elix" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
+    <sheet name="sheet8" sheetId="9" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Elix" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="167">
   <si>
     <t>Table: Descriptive statistics</t>
   </si>
@@ -506,12 +508,6 @@
     <t>51 (0.4%)</t>
   </si>
   <si>
-    <t>YEAR</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
     <t>Primary</t>
   </si>
   <si>
@@ -522,16 +518,49 @@
   </si>
   <si>
     <t>Arthritis, type unspecified</t>
+  </si>
+  <si>
+    <t>Cefadroxil</t>
+  </si>
+  <si>
+    <t>Cefdinir</t>
+  </si>
+  <si>
+    <t>Cephalexin</t>
+  </si>
+  <si>
+    <t>Clindamycin</t>
+  </si>
+  <si>
+    <t>Doxycycline</t>
+  </si>
+  <si>
+    <t>TMP_SMX</t>
+  </si>
+  <si>
+    <t>Percent of EOA Cases</t>
+  </si>
+  <si>
+    <t>Antibiotic</t>
+  </si>
+  <si>
+    <t>EOA Rate</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +642,44 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -634,7 +701,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -707,12 +774,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -834,14 +911,42 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1154,6 +1259,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C81CFE-16EE-455C-9C17-AC390FBD5FF7}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G6:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="49">
+        <v>2848</v>
+      </c>
+      <c r="C2" s="50">
+        <v>0.21887487999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="49">
+        <v>206</v>
+      </c>
+      <c r="C3" s="50">
+        <v>1.5831540000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="49">
+        <v>5281</v>
+      </c>
+      <c r="C4" s="50">
+        <v>0.40585612999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="49">
+        <v>753</v>
+      </c>
+      <c r="C5" s="50">
+        <v>5.7869660000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="49">
+        <v>1297</v>
+      </c>
+      <c r="C6" s="50">
+        <v>9.9677219999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="49">
+        <v>2627</v>
+      </c>
+      <c r="C7" s="50">
+        <v>0.20189056</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85FD749-F70E-47E4-90A1-550E88201E21}">
   <dimension ref="C4:G20"/>
   <sheetViews>
@@ -1308,7 +1510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9421064-70D7-4334-B25B-96DFE06AACC1}">
   <dimension ref="B5:I21"/>
   <sheetViews>
@@ -1698,7 +1900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72755CAE-3C7F-47C8-B77F-3DF95A26F09C}">
   <dimension ref="C8:J43"/>
   <sheetViews>
@@ -1977,7 +2179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7194ED90-6E35-455B-843C-C1C0BDBC4B49}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -2391,7 +2593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E136CD-2CFE-4539-BB73-23E84B8435E1}">
   <dimension ref="B6:F20"/>
   <sheetViews>
@@ -2645,12 +2847,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4966FD-1D6D-4A84-812B-352D48CD3902}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,472 +3181,517 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4464D4A-37E4-4425-8740-6C871D1B96A5}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+    <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="56"/>
+      <c r="B1" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="I1" s="48"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="I1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="60" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G2" s="60" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="I2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="I2" s="60" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
         <v>2009</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="61">
         <v>46619</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="62">
         <v>9.9699999999999997E-3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="61">
         <v>13</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="62">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="61">
         <v>88</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="62">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="61">
         <v>21459</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="62">
         <v>7.3600000000000002E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
         <v>2010</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="61">
         <v>48667</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="62">
         <v>1.03E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="61">
         <v>14</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="62">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="61">
         <v>73</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="62">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="61">
         <v>21527</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="62">
         <v>9.8899999999999995E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
         <v>2011</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="61">
         <v>52850</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="62">
         <v>8.8199999999999997E-3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="61">
         <v>14</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="62">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="61">
         <v>99</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="62">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="61">
         <v>23583</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="62">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
         <v>2012</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="61">
         <v>51589</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="62">
         <v>0.01</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="61">
         <v>10</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="62">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="61">
         <v>83</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="62">
         <v>1.2E-2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="61">
         <v>23657</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="62">
         <v>9.1699999999999993E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
         <v>2013</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="61">
         <v>43253</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="62">
         <v>9.7099999999999999E-3</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="61">
         <v>8</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="62">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="61">
         <v>93</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="62">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="61">
         <v>20639</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="62">
         <v>9.9799999999999993E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
         <v>2014</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="61">
         <v>44255</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="62">
         <v>9.4500000000000001E-3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="61">
         <v>5</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="62">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="61">
         <v>127</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="62">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="61">
         <v>21050</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="62">
         <v>1.04E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
         <v>2015</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="61">
         <v>33526</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="62">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="61">
         <v>9</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="62">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="61">
         <v>56</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="62">
         <v>1.7899999999999999E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="61">
         <v>9379</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="62">
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="12">
         <v>2016</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="61">
         <v>50992</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="62">
         <v>1.35E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="61">
         <v>17</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="62">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="61">
         <v>40</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="62">
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="61">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="12">
         <v>2017</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="61">
         <v>43686</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="62">
         <v>1.6500000000000001E-2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="61">
         <v>25</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="62">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="61">
         <v>30</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="62">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="61">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="12">
         <v>2018</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="61">
         <v>41792</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="62">
         <v>2.3900000000000001E-2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="61">
         <v>20</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="62">
         <v>0.05</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="61">
         <v>42</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="62">
         <v>0</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="61">
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="12">
         <v>2019</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="61">
         <v>32214</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="62">
         <v>3.3399999999999999E-2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="61">
         <v>25</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="62">
         <v>0.08</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="61">
         <v>17</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="62">
         <v>0.23499999999999999</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="61">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
         <v>2020</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="61">
         <v>30357</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="62">
         <v>4.58E-2</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="61">
         <v>17</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="62">
         <v>0.17599999999999999</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="61">
         <v>15</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="62">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="61">
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
         <v>2021</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="61">
         <v>34654</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="62">
         <v>6.6500000000000004E-2</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="61">
         <v>19</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="62">
         <v>5.2600000000000001E-2</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="61">
         <v>21</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="62">
         <v>0.19</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="61">
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
         <v>2022</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="61">
         <v>16130</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="62">
         <v>7.9500000000000001E-2</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="61">
         <v>11</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="62">
         <v>0.182</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="61">
         <v>8</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="62">
         <v>0.125</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="61">
         <v>0</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="12">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="63">
+        <f>SUM(B3:B16)</f>
+        <v>570584</v>
+      </c>
+      <c r="C17" s="56"/>
+      <c r="D17" s="63">
+        <f>SUM(D3:D16)</f>
+        <v>207</v>
+      </c>
+      <c r="E17" s="56"/>
+      <c r="F17" s="63">
+        <f>SUM(F3:F16)</f>
+        <v>792</v>
+      </c>
+      <c r="G17" s="56"/>
+      <c r="H17" s="63">
+        <f>SUM(H3:H16)</f>
+        <v>141294</v>
+      </c>
+      <c r="I17" s="56"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I21" s="47"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>B17/SUM(B17,D17,F17,H17,)</f>
+        <v>0.80039614126981229</v>
+      </c>
+      <c r="C23" s="55">
+        <f>B17/712212</f>
+        <v>0.80114347975041145</v>
       </c>
     </row>
   </sheetData>
@@ -3457,4 +3704,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCC79AB-F332-436B-A51C-5DFCBC80FA57}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="49">
+        <v>5281</v>
+      </c>
+      <c r="C2" s="50">
+        <v>0.40585612999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="49">
+        <v>2848</v>
+      </c>
+      <c r="C3" s="50">
+        <v>0.21887487999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="49">
+        <v>2627</v>
+      </c>
+      <c r="C4" s="50">
+        <v>0.20189056</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="49">
+        <v>1297</v>
+      </c>
+      <c r="C5" s="50">
+        <v>9.9677219999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="49">
+        <v>753</v>
+      </c>
+      <c r="C6" s="50">
+        <v>5.7869660000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="49">
+        <v>206</v>
+      </c>
+      <c r="C7" s="50">
+        <v>1.5831540000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:C7">
+    <sortCondition descending="1" ref="C2:C7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>